<commit_message>
KIBON-63: Lastenausgleich. Text-Spalten im Excel links ausgerichtet, Übersetzung des Jobs hinzugefügt
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichKibon.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichKibon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beim\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\M$\hefr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439D7D5C-D263-4E16-8571-07782AC3F07A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4573D8C-3BA0-4DAF-B68D-D5D8D40F9009}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6D37441E-09CE-4F94-BF5A-8FAE3F6E6CF7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{6D37441E-09CE-4F94-BF5A-8FAE3F6E6CF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -282,24 +282,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -312,6 +294,27 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -628,9 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFD2C01-3190-4613-9E97-C1D328FAAE82}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -668,91 +669,91 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="O6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="P6" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="R6" s="16" t="s">
+      <c r="R6" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="17"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="19"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -770,13 +771,13 @@
       <c r="G8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="24" t="s">
         <v>23</v>
       </c>
       <c r="K8" s="4" t="s">
@@ -793,11 +794,11 @@
         <f t="shared" ref="N8" si="0">EOMONTH(E8,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O8" s="19" t="e">
+      <c r="O8" s="13" t="e">
         <f>N8-M8+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P8" s="19" t="e">
+      <c r="P8" s="13" t="e">
         <f>F8-E8+1</f>
         <v>#VALUE!</v>
       </c>
@@ -805,7 +806,7 @@
         <f>P8/O8</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R8" s="20" t="e">
+      <c r="R8" s="14" t="e">
         <f>G8*Q8/12</f>
         <v>#VALUE!</v>
       </c>
@@ -834,7 +835,7 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
-      <c r="R9" s="21" t="e">
+      <c r="R9" s="15" t="e">
         <f>SUM(anteil)</f>
         <v>#VALUE!</v>
       </c>
@@ -843,7 +844,7 @@
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="22" t="e">
+      <c r="C11" s="16" t="e">
         <f>L9/R9</f>
         <v>#VALUE!</v>
       </c>
@@ -852,23 +853,13 @@
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="22" t="e">
+      <c r="C12" s="16" t="e">
         <f>C11*0.2</f>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="A6:A7"/>
@@ -877,6 +868,16 @@
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
directToDev: Währungsformate für Lastenausgleich Report angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichKibon.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichKibon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\M$\hefr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egch\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4573D8C-3BA0-4DAF-B68D-D5D8D40F9009}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74DC510-6DC7-47CC-97DA-D6D8086D7F42}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{6D37441E-09CE-4F94-BF5A-8FAE3F6E6CF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{6D37441E-09CE-4F94-BF5A-8FAE3F6E6CF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0"/>
+    <numFmt numFmtId="167" formatCode="[$CHF-807]\ #,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -253,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -264,13 +264,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -290,31 +284,38 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -669,91 +670,91 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="P6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="19"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="21"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -771,19 +772,19 @@
       <c r="G8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="J8" s="15" t="s">
         <v>23</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="22" t="s">
         <v>25</v>
       </c>
       <c r="M8" s="4" t="e">
@@ -794,19 +795,19 @@
         <f t="shared" ref="N8" si="0">EOMONTH(E8,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O8" s="13" t="e">
+      <c r="O8" s="11" t="e">
         <f>N8-M8+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P8" s="13" t="e">
+      <c r="P8" s="11" t="e">
         <f>F8-E8+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q8" s="10" t="e">
+      <c r="Q8" s="8" t="e">
         <f>P8/O8</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R8" s="14" t="e">
+      <c r="R8" s="12" t="e">
         <f>G8*Q8/12</f>
         <v>#VALUE!</v>
       </c>
@@ -815,36 +816,39 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8">
+      <c r="A9" s="6"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="23">
         <f>SUM(gutschein)</f>
         <v>0</v>
       </c>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="15" t="e">
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="13" t="e">
         <f>SUM(anteil)</f>
         <v>#VALUE!</v>
       </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L10" s="25"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="16" t="e">
+      <c r="C11" s="24" t="e">
         <f>L9/R9</f>
         <v>#VALUE!</v>
       </c>
@@ -853,13 +857,18 @@
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="16" t="e">
+      <c r="C12" s="24" t="e">
         <f>C11*0.2</f>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="A6:A7"/>
@@ -873,11 +882,6 @@
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>